<commit_message>
adding recent NGF runs to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llin\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4095D7B-8C91-4BA4-A21F-FBA27C87C5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E8AEC-E809-448F-9D83-16BDC32C01B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="70" yWindow="1140" windowWidth="22490" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>category</t>
   </si>
@@ -68,9 +68,6 @@
     <t>2015_TM152_IPA_17</t>
   </si>
   <si>
-    <t>"census_petrale"</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
@@ -123,6 +120,54 @@
   </si>
   <si>
     <t>https://app.asana.com/0/0/1206123647391998/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP03_Path1_01</t>
+  </si>
+  <si>
+    <t>P1_AllLaneTolling</t>
+  </si>
+  <si>
+    <t>R2_ALT</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NGFround2_P1_01</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>P1 initial run -  carpool and tolls.csv fixes</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_01</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_02</t>
+  </si>
+  <si>
+    <t>P1 initial run -  tolls not in 2000$</t>
+  </si>
+  <si>
+    <t>P1 initial run -  complete street fixes</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_02_MinTollOff</t>
+  </si>
+  <si>
+    <t>P1 initial run -  test with min toll turned off</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1207102772074759/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1207177908266953/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1206539107762749/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1201809392759895/1207151709274835/f</t>
   </si>
 </sst>
 </file>
@@ -294,9 +339,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -334,7 +379,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -440,7 +485,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -582,7 +627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -590,11 +635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -617,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -626,16 +671,16 @@
         <v>0</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>7</v>
@@ -658,10 +703,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -669,77 +714,207 @@
         <v>10</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="8">
         <v>2035</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8">
         <v>2035</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>26</v>
-      </c>
       <c r="F4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>11</v>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
copying pathway 4, 1x 1a and 1b from round 1
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one-master\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalatorre\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E8AEC-E809-448F-9D83-16BDC32C01B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970216B9-260F-4835-9295-1385930D4A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70" yWindow="1140" windowWidth="22490" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26925" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
   <si>
     <t>category</t>
   </si>
@@ -168,13 +168,91 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1201809392759895/1207151709274835/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_01</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_01_AOCx1.25_v2</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_03_pretollcalib</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP10_Path1a_02</t>
+  </si>
+  <si>
+    <t>NGF</t>
+  </si>
+  <si>
+    <t>Pathway 1a</t>
+  </si>
+  <si>
+    <t>Pathway 1a - All Lane Tolling + Transit Double Down</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P1a_AllLaneTolling_ImproveTransit_09</t>
+  </si>
+  <si>
+    <t>Rerun Pathway 1a with new network</t>
+  </si>
+  <si>
+    <t>"Final Blueprint runs\Final Blueprint (s24)\BAUS v2.25 - FINAL VERSION"</t>
+  </si>
+  <si>
+    <t>run182</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP10_Path1b_02</t>
+  </si>
+  <si>
+    <t>Pathway 1b</t>
+  </si>
+  <si>
+    <t>Pathway 1b - All Lane Tolling + Affordable</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P1b_AllLaneTolling_Affordable_04</t>
+  </si>
+  <si>
+    <t>Rerun Pathway 1b with new network</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP10_Path1x_01</t>
+  </si>
+  <si>
+    <t>Pathway 1x</t>
+  </si>
+  <si>
+    <t>Pathway 1x - All-lane tolling pricing strategy only</t>
+  </si>
+  <si>
+    <t>NGF_Network_P1x_AllLaneTolling_PricingOnly_01</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1201809392759895/1205309291141002/f</t>
+  </si>
+  <si>
+    <t>2035_TM152_NGF_NP10_Path4_02</t>
+  </si>
+  <si>
+    <t>Pathway 4</t>
+  </si>
+  <si>
+    <t>Pathway 4 - No New Pricing</t>
+  </si>
+  <si>
+    <t>NGF_Networks_P4_NoNewPricing_03</t>
+  </si>
+  <si>
+    <t>Rerun Pathway 4 with new network</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -228,8 +306,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +333,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -258,13 +361,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -284,8 +388,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{564E6A42-6173-40A4-9CC8-4130B69477E9}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{CC352229-7B38-4835-9297-CE7CE23BF08B}"/>
@@ -635,11 +759,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -647,9 +771,10 @@
     <col min="1" max="1" width="12.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="13.09765625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="22.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.296875" customWidth="1"/>
     <col min="8" max="8" width="47.3984375" customWidth="1"/>
+    <col min="9" max="9" width="59.69921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.69921875" customWidth="1"/>
     <col min="11" max="11" width="15" style="10" customWidth="1"/>
   </cols>
@@ -901,6 +1026,9 @@
       <c r="F8" t="s">
         <v>39</v>
       </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
       <c r="H8" t="s">
         <v>31</v>
       </c>
@@ -914,9 +1042,203 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="10">
+        <v>2035</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12">
+        <v>2035</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20">
+        <v>2035</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="12">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I14" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fill in category for no project runs
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalatorre\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970216B9-260F-4835-9295-1385930D4A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08D9498-7070-4276-B1AF-E342D2849CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26925" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
   <si>
     <t>category</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Rerun Pathway 4 with new network</t>
+  </si>
+  <si>
+    <t>NoProject</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1055,6 +1058,9 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
       <c r="G9" t="s">
         <v>32</v>
       </c>
@@ -1072,6 +1078,9 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
       <c r="G10" t="s">
         <v>32</v>
       </c>
@@ -1088,6 +1097,9 @@
       </c>
       <c r="D11" t="s">
         <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
       </c>
       <c r="G11" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
add Path4_02_pretollcalib the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B7D8AA-4EAA-4124-B903-D78AD958465C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413248D5-AA18-4E47-A921-AE397240F822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="121">
   <si>
     <t>category</t>
   </si>
@@ -350,9 +350,6 @@
     <t>P6 toll-calibration run</t>
   </si>
   <si>
-    <t>P6_EL_DoubleEL</t>
-  </si>
-  <si>
     <t>switched from P6_11 to P6_13</t>
   </si>
   <si>
@@ -390,6 +387,18 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1203644633064654/1206322696359485/f</t>
+  </si>
+  <si>
+    <t>P6_EL_DualEL</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path4_02_pretollcalib</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NGFround2_P4_09</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/572982923864207/1207634640713913/f</t>
   </si>
 </sst>
 </file>
@@ -517,7 +526,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -557,22 +566,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -941,11 +946,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -996,237 +1001,237 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>2015</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="J2" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="J2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C4" s="21" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="24">
-        <v>2035</v>
-      </c>
-      <c r="C5" s="21" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="23">
+        <v>2035</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C6" s="21" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C7" s="21" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="21" t="s">
+      <c r="D7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="20">
-        <v>2035</v>
-      </c>
-      <c r="C8" s="21" t="s">
+      <c r="J7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="19">
+        <v>2035</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="21" t="s">
+      <c r="D8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21" t="s">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="22" t="s">
+      <c r="J8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1494,7 +1499,7 @@
         <v>2035</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>19</v>
@@ -1503,13 +1508,13 @@
         <v>69</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>10</v>
@@ -1526,7 +1531,7 @@
         <v>2035</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>19</v>
@@ -1535,13 +1540,13 @@
         <v>69</v>
       </c>
       <c r="F18" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I18" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="J18" s="13" t="s">
         <v>10</v>
@@ -1558,7 +1563,7 @@
         <v>2035</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>19</v>
@@ -1567,16 +1572,16 @@
         <v>69</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>10</v>
@@ -1649,131 +1654,163 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="28">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="29" t="s">
+    <row r="22" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="27" t="s">
+      <c r="D23" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F23" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H23" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="I23" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="28">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="29" t="s">
+      <c r="J23" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C24" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="27" t="s">
+      <c r="D24" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F24" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H24" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="I23" s="29" t="s">
+      <c r="I24" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="J23" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="K23" s="30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C24" s="33" t="s">
+      <c r="J24" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C25" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="31" t="s">
+      <c r="D25" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H24" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="I24" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="J24" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="K24" s="34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="32">
-        <v>2035</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="H25" s="33" t="s">
+      <c r="I26" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I25" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="J25" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="K25" s="34" t="s">
+      <c r="J26" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="32" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add column with mapped paths for model3-a
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalatorre\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E04246-E58A-4972-9BBA-C02FB6399333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD00328-93DB-4DA1-B73C-88192C3F2EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="1620" windowWidth="24750" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="141">
   <si>
     <t>category</t>
   </si>
@@ -426,6 +426,39 @@
   </si>
   <si>
     <t>https://app.asana.com/0/0/1207636747806736/f</t>
+  </si>
+  <si>
+    <t>path_on_model3-a</t>
+  </si>
+  <si>
+    <t>A:\\Projects\\2035_TM160_NGFr2_NP04_Path1_02</t>
+  </si>
+  <si>
+    <t>A:\\Projects\\2035_TM160_NGFr2_NP04_Path4_01</t>
+  </si>
+  <si>
+    <t>G:\\Projects\\2035_TM160_NGF_r2_NoProject_01</t>
+  </si>
+  <si>
+    <t>B:\\Projects\\2035_TM160_NGF_r2_NoProject_04</t>
+  </si>
+  <si>
+    <t>F:\\Projects\\2035_TM160_NGFr2_NP04_Path5_01</t>
+  </si>
+  <si>
+    <t>H:\\Projects\\2035_TM160_NGFr2_NP04_Path6_01</t>
+  </si>
+  <si>
+    <t>X:\\Projects\\2035_TM152_NGF_NP10_Path1a_02</t>
+  </si>
+  <si>
+    <t>B:\\Projects\\2035_TM152_NGF_NP10_Path1b_02</t>
+  </si>
+  <si>
+    <t>A:\\Projects\\2035_TM152_NGF_NP10_Path1x_01</t>
+  </si>
+  <si>
+    <t>G:\\Projects\\2035_TM152_NGF_NP10_Path4_02</t>
   </si>
 </sst>
 </file>
@@ -973,27 +1006,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.3984375" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" customWidth="1"/>
+    <col min="5" max="5" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.296875" customWidth="1"/>
+    <col min="8" max="8" width="47.3984375" customWidth="1"/>
+    <col min="9" max="9" width="59.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.69921875" style="14" customWidth="1"/>
     <col min="11" max="11" width="15" style="14" customWidth="1"/>
+    <col min="12" max="12" width="44.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1027,8 +1061,11 @@
       <c r="K1" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1056,7 +1093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1090,8 +1127,11 @@
       <c r="K3" s="21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1125,8 +1165,11 @@
       <c r="K4" s="21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1160,8 +1203,11 @@
       <c r="K5" s="14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1195,8 +1241,11 @@
       <c r="K6" s="21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1229,7 +1278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1262,7 +1311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1294,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1326,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1360,8 +1409,11 @@
       <c r="K11" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L11" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1393,7 +1445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -1425,7 +1477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -1456,8 +1508,11 @@
       <c r="K14" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L14" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1486,7 +1541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
@@ -1518,7 +1573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
@@ -1550,7 +1605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
@@ -1582,7 +1637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
@@ -1616,8 +1671,11 @@
       <c r="K19" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L19" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>13</v>
       </c>
@@ -1649,7 +1707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>13</v>
       </c>
@@ -1681,7 +1739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>13</v>
       </c>
@@ -1713,7 +1771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>13</v>
       </c>
@@ -1744,8 +1802,11 @@
       <c r="K23" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L23" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>13</v>
       </c>
@@ -1777,7 +1838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>13</v>
       </c>
@@ -1809,7 +1870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>13</v>
       </c>
@@ -1840,8 +1901,11 @@
       <c r="K26" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L26" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>13</v>
       </c>
@@ -1873,7 +1937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
         <v>13</v>
       </c>
@@ -1905,7 +1969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
         <v>13</v>
       </c>
@@ -1936,8 +2000,12 @@
       <c r="K29" s="32" t="s">
         <v>10</v>
       </c>
+      <c r="L29" s="31" t="s">
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L29" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I5" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>

</xml_diff>

<commit_message>
Revert "remove double slashes"
This reverts commit ac54a298c82c94f80a69bcf3c2fd52fd7ced3edf.
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalatorre\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB26F1-8B3D-40D2-9043-F2C8801CD7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA69430-D4CE-4207-AE52-FE405EEF2286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,6 +431,24 @@
     <t>path_on_model3-a</t>
   </si>
   <si>
+    <t>A:\\Projects\\2035_TM160_NGFr2_NP04_Path1_02</t>
+  </si>
+  <si>
+    <t>A:\\Projects\\2035_TM160_NGFr2_NP04_Path4_01</t>
+  </si>
+  <si>
+    <t>G:\\Projects\\2035_TM160_NGF_r2_NoProject_01</t>
+  </si>
+  <si>
+    <t>B:\\Projects\\2035_TM160_NGF_r2_NoProject_04</t>
+  </si>
+  <si>
+    <t>F:\\Projects\\2035_TM160_NGFr2_NP04_Path5_01</t>
+  </si>
+  <si>
+    <t>H:\\Projects\\2035_TM160_NGFr2_NP04_Path6_01</t>
+  </si>
+  <si>
     <t>X:\\Projects\\2035_TM152_NGF_NP10_Path1a_02</t>
   </si>
   <si>
@@ -476,31 +494,13 @@
     <t>2035_TM160_NGFr2_NP04_Path6_02</t>
   </si>
   <si>
+    <t>H:\\Projects\\2035_TM160_NGFr2_NP04_Path6_02</t>
+  </si>
+  <si>
     <t>to become current</t>
   </si>
   <si>
     <t>may not need to run this</t>
-  </si>
-  <si>
-    <t>A:\Projects\2035_TM160_NGFr2_NP04_Path1_02</t>
-  </si>
-  <si>
-    <t>G:\Projects\2035_TM160_NGF_r2_NoProject_01</t>
-  </si>
-  <si>
-    <t>B:\Projects\2035_TM160_NGF_r2_NoProject_04</t>
-  </si>
-  <si>
-    <t>A:\Projects\2035_TM160_NGFr2_NP04_Path4_01</t>
-  </si>
-  <si>
-    <t>F:\Projects\2035_TM160_NGFr2_NP04_Path5_01</t>
-  </si>
-  <si>
-    <t>H:\Projects\2035_TM160_NGFr2_NP04_Path6_01</t>
-  </si>
-  <si>
-    <t>H:\Projects\2035_TM160_NGFr2_NP04_Path6_02</t>
   </si>
 </sst>
 </file>
@@ -1055,9 +1055,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1175,7 +1175,7 @@
         <v>53</v>
       </c>
       <c r="L3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1213,7 +1213,7 @@
         <v>53</v>
       </c>
       <c r="L4" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1251,7 +1251,7 @@
         <v>53</v>
       </c>
       <c r="L5" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
         <v>53</v>
       </c>
       <c r="L6" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1457,7 +1457,7 @@
         <v>10</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1556,7 +1556,7 @@
         <v>10</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1719,7 +1719,7 @@
         <v>10</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1821,7 +1821,7 @@
         <v>10</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1841,7 +1841,7 @@
         <v>91</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H23" s="15" t="s">
         <v>119</v>
@@ -1864,7 +1864,7 @@
         <v>2035</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>19</v>
@@ -1873,7 +1873,7 @@
         <v>91</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>119</v>
@@ -1896,7 +1896,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>19</v>
@@ -1908,7 +1908,7 @@
         <v>126</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>119</v>
@@ -1921,7 +1921,7 @@
         <v>10</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
@@ -2011,7 +2011,7 @@
         <v>31</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="I28" s="27" t="s">
         <v>125</v>
@@ -2023,7 +2023,7 @@
         <v>10</v>
       </c>
       <c r="L28" s="27" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -2113,7 +2113,7 @@
         <v>31</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="I31" s="29" t="s">
         <v>128</v>
@@ -2125,7 +2125,7 @@
         <v>10</v>
       </c>
       <c r="L31" s="29" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -2136,7 +2136,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>19</v>
@@ -2148,10 +2148,10 @@
         <v>102</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="J32" s="31" t="s">
         <v>10</v>
@@ -2168,7 +2168,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D33" s="29" t="s">
         <v>19</v>
@@ -2180,7 +2180,7 @@
         <v>103</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="J33" s="31" t="s">
         <v>10</v>
@@ -2197,7 +2197,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>19</v>
@@ -2209,10 +2209,10 @@
         <v>127</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="J34" s="31" t="s">
         <v>10</v>
@@ -2221,7 +2221,7 @@
         <v>10</v>
       </c>
       <c r="L34" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added two pathway 1 test runs to model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bayareametro-my.sharepoint.com/personal/atapase_bayareametro_gov/Documents/Documents/GitHub/travel-model-one/utilities/NextGenFwys/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{5DA69430-D4CE-4207-AE52-FE405EEF2286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7120BBAE-7B3B-43FB-8B8A-793155CC0726}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF99B38-FEBF-4BA7-B7FC-DC004E0A3FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="161">
   <si>
     <t>category</t>
   </si>
@@ -498,6 +498,27 @@
   </si>
   <si>
     <t>may not need to run this</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_03</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_04</t>
+  </si>
+  <si>
+    <t>P1 initial run -  vision zero test</t>
+  </si>
+  <si>
+    <t>P1 initial run -  tolls creation test</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NGFround2_P1_04</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1207713742308166/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1207731071720316/f</t>
   </si>
 </sst>
 </file>
@@ -1050,28 +1071,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.3984375" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" customWidth="1"/>
+    <col min="5" max="5" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.296875" customWidth="1"/>
+    <col min="8" max="8" width="47.3984375" customWidth="1"/>
+    <col min="9" max="9" width="59.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.69921875" style="14" customWidth="1"/>
     <col min="11" max="11" width="15" style="14" customWidth="1"/>
-    <col min="12" max="12" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1130,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1175,7 +1196,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1213,7 +1234,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1251,7 +1272,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1289,7 +1310,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1322,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1355,7 +1376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1387,7 +1408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1419,7 +1440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1438,9 +1459,6 @@
       <c r="F11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="H11" s="4" t="s">
         <v>30</v>
       </c>
@@ -1457,7 +1475,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1489,7 +1507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -1521,76 +1539,82 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C14" s="7" t="s">
+    <row r="14" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>19</v>
@@ -1599,13 +1623,10 @@
         <v>69</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>10</v>
@@ -1613,8 +1634,11 @@
       <c r="K16" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L16" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1646,7 @@
         <v>2035</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>19</v>
@@ -1631,13 +1655,10 @@
         <v>69</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>10</v>
@@ -1646,7 +1667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
@@ -1654,7 +1675,7 @@
         <v>2035</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>19</v>
@@ -1663,13 +1684,13 @@
         <v>69</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="J18" s="13" t="s">
         <v>10</v>
@@ -1678,7 +1699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
@@ -1686,7 +1707,7 @@
         <v>2035</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>19</v>
@@ -1695,100 +1716,100 @@
         <v>69</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I19" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="J19" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L19" s="7" t="s">
+      <c r="J21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C20" s="15" t="s">
+    <row r="22" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>122</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>19</v>
@@ -1797,16 +1818,13 @@
         <v>91</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="J22" s="17" t="s">
         <v>10</v>
@@ -1814,11 +1832,8 @@
       <c r="K22" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L22" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>13</v>
       </c>
@@ -1826,7 +1841,7 @@
         <v>2035</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>19</v>
@@ -1835,13 +1850,13 @@
         <v>91</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J23" s="17" t="s">
         <v>10</v>
@@ -1850,7 +1865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>13</v>
       </c>
@@ -1858,7 +1873,7 @@
         <v>2035</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>19</v>
@@ -1867,13 +1882,16 @@
         <v>91</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>119</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="J24" s="17" t="s">
         <v>10</v>
@@ -1881,8 +1899,11 @@
       <c r="K24" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L24" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>13</v>
       </c>
@@ -1890,7 +1911,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>19</v>
@@ -1899,98 +1920,98 @@
         <v>91</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="18" t="s">
+        <v>120</v>
+      </c>
       <c r="J25" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K25" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="15" t="s">
+    </row>
+    <row r="26" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="27" t="s">
+    <row r="28" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C28" s="27" t="s">
         <v>89</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H26" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="I26" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J26" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K26" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="I27" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="J27" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K27" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>123</v>
       </c>
       <c r="D28" s="25" t="s">
         <v>19</v>
@@ -1999,100 +2020,100 @@
         <v>92</v>
       </c>
       <c r="F28" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J29" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G28" s="27" t="s">
+      <c r="G30" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="27" t="s">
+      <c r="H30" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I28" s="27" t="s">
+      <c r="I30" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="J28" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K28" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L28" s="27" t="s">
+      <c r="J30" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="27" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="29" t="s">
+    <row r="31" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="29" t="s">
         <v>99</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H29" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="J29" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K29" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I30" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K30" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>121</v>
       </c>
       <c r="D31" s="29" t="s">
         <v>19</v>
@@ -2101,13 +2122,13 @@
         <v>117</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="I31" s="29" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J31" s="31" t="s">
         <v>10</v>
@@ -2115,11 +2136,8 @@
       <c r="K31" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L31" s="29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29" t="s">
         <v>13</v>
       </c>
@@ -2127,7 +2145,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>19</v>
@@ -2136,13 +2154,13 @@
         <v>117</v>
       </c>
       <c r="F32" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="J32" s="31" t="s">
         <v>10</v>
@@ -2151,7 +2169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
         <v>13</v>
       </c>
@@ -2159,7 +2177,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D33" s="29" t="s">
         <v>19</v>
@@ -2168,10 +2186,13 @@
         <v>117</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="I33" s="29" t="s">
+        <v>128</v>
       </c>
       <c r="J33" s="31" t="s">
         <v>10</v>
@@ -2179,8 +2200,11 @@
       <c r="K33" s="31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L33" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29" t="s">
         <v>13</v>
       </c>
@@ -2188,7 +2212,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>19</v>
@@ -2197,31 +2221,92 @@
         <v>117</v>
       </c>
       <c r="F34" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="H34" s="29" t="s">
         <v>143</v>
       </c>
+      <c r="I34" s="29" t="s">
+        <v>144</v>
+      </c>
       <c r="J34" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K34" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L34" s="29" t="s">
+    </row>
+    <row r="35" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J36" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L36" s="29" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L31" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L33" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I5" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
     <hyperlink ref="I12" r:id="rId2" xr:uid="{088533EE-4DDB-4145-8A51-9A459A5B0EE7}"/>
-    <hyperlink ref="I20" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
+    <hyperlink ref="I22" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
added a pair of Path1 runs for Fwy FSS assessment to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF99B38-FEBF-4BA7-B7FC-DC004E0A3FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1092A34B-A0E2-46E1-AB64-B2EEC74AA19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="21590" windowHeight="13010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="169">
   <si>
     <t>category</t>
   </si>
@@ -519,6 +519,30 @@
   </si>
   <si>
     <t>https://app.asana.com/0/0/1207731071720316/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_05</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_06</t>
+  </si>
+  <si>
+    <t>P1 - base run for Fwy FFS assessment</t>
+  </si>
+  <si>
+    <t>P1 - proj run for Fwy FFS assessment</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NGFround2_P1_05</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NGFround2_P1_06</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/572982923864207/1207750211446447/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/572982923864207/1207750211446449/f</t>
   </si>
 </sst>
 </file>
@@ -1071,11 +1095,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1590,9 +1614,6 @@
       <c r="F15" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="H15" s="4" t="s">
         <v>158</v>
       </c>
@@ -1606,64 +1627,73 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="13" t="s">
+    <row r="16" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1675,7 +1705,7 @@
         <v>2035</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>19</v>
@@ -1684,19 +1714,19 @@
         <v>69</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J18" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>10</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1707,7 +1737,7 @@
         <v>2035</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>19</v>
@@ -1716,13 +1746,10 @@
         <v>69</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>10</v>
@@ -1739,7 +1766,7 @@
         <v>2035</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>19</v>
@@ -1748,13 +1775,13 @@
         <v>69</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="J20" s="13" t="s">
         <v>10</v>
@@ -1771,7 +1798,7 @@
         <v>2035</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>19</v>
@@ -1780,89 +1807,89 @@
         <v>69</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="J21" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L21" s="7" t="s">
+      <c r="J23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="7" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1873,7 +1900,7 @@
         <v>2035</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>19</v>
@@ -1882,25 +1909,19 @@
         <v>91</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="J24" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="L24" s="15" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1911,7 +1932,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>19</v>
@@ -1920,13 +1941,13 @@
         <v>91</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J25" s="17" t="s">
         <v>10</v>
@@ -1943,7 +1964,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>19</v>
@@ -1952,19 +1973,25 @@
         <v>91</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="H26" s="15" t="s">
         <v>119</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="J26" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K26" s="17" t="s">
         <v>10</v>
+      </c>
+      <c r="L26" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1975,7 +2002,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>19</v>
@@ -1984,87 +2011,87 @@
         <v>91</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H27" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I27" s="18"/>
+      <c r="I27" s="18" t="s">
+        <v>120</v>
+      </c>
       <c r="J27" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L27" s="15" t="s">
+    </row>
+    <row r="28" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="15" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H28" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="I28" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J28" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K28" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="H29" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="I29" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="J29" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K29" s="28" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
@@ -2075,7 +2102,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>19</v>
@@ -2084,89 +2111,89 @@
         <v>92</v>
       </c>
       <c r="F30" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="J30" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G32" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H30" s="27" t="s">
+      <c r="H32" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I30" s="27" t="s">
+      <c r="I32" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="J30" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K30" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L30" s="27" t="s">
+      <c r="J32" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" s="27" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="I31" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="J31" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K31" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I32" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="J32" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="31" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -2177,7 +2204,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="D33" s="29" t="s">
         <v>19</v>
@@ -2186,22 +2213,19 @@
         <v>117</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="I33" s="29" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J33" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K33" s="31" t="s">
         <v>10</v>
-      </c>
-      <c r="L33" s="29" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -2212,7 +2236,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>19</v>
@@ -2221,13 +2245,13 @@
         <v>117</v>
       </c>
       <c r="F34" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="J34" s="31" t="s">
         <v>10</v>
@@ -2244,7 +2268,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D35" s="29" t="s">
         <v>19</v>
@@ -2253,16 +2277,22 @@
         <v>117</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="I35" s="29" t="s">
+        <v>128</v>
       </c>
       <c r="J35" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K35" s="31" t="s">
         <v>10</v>
+      </c>
+      <c r="L35" s="29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -2273,7 +2303,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>19</v>
@@ -2282,31 +2312,92 @@
         <v>117</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="H36" s="29" t="s">
         <v>143</v>
       </c>
+      <c r="I36" s="29" t="s">
+        <v>144</v>
+      </c>
       <c r="J36" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K36" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L36" s="29" t="s">
+    </row>
+    <row r="37" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K38" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L38" s="29" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L33" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L35" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I5" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
     <hyperlink ref="I12" r:id="rId2" xr:uid="{088533EE-4DDB-4145-8A51-9A459A5B0EE7}"/>
-    <hyperlink ref="I22" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
+    <hyperlink ref="I24" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
update NGF Round 2 run log with latest runs
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atapase\OneDrive - Metropolitan Transportation Commission\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C897DB98-2137-4F01-8ED0-E6A9CC515284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE17D2D4-0959-4F59-B3BF-0729BF8207EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="245">
   <si>
     <t>category</t>
   </si>
@@ -705,13 +705,79 @@
   </si>
   <si>
     <t>B:\\Projects\\2035_TM160_NGF_r2_NoProject_04_add5.9c</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path2_01</t>
+  </si>
+  <si>
+    <t>P2_MBUF</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NGFround2_P1_14_NoVisionZero</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1207994963427970/f</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_05</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1207994951064423/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_12_40c10c</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>P1 - 40c/10c - no local road spd limit red</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_05_mbuf4.4cTest</t>
+  </si>
+  <si>
+    <t>NP run - no EL</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1207994963427971/f</t>
+  </si>
+  <si>
+    <t>to be started</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_12_50c10c</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_12_30c15c</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_05_add4.4c</t>
+  </si>
+  <si>
+    <t>NP run - no EL, AOC+4.4c</t>
+  </si>
+  <si>
+    <t>NP run - no EL, MBUF at 4.4c</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path2_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2 - MBUF at 7.5c (same toll cap as P1_12) </t>
+  </si>
+  <si>
+    <t>P2 - MBUF at 7.5c (try a lower cap, assuming the average household make 4 trips a day)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -783,8 +849,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -821,6 +893,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -838,7 +916,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -905,6 +983,16 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1257,29 +1345,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.3984375" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" customWidth="1"/>
+    <col min="5" max="5" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.19921875" customWidth="1"/>
+    <col min="8" max="8" width="47.3984375" customWidth="1"/>
+    <col min="9" max="9" width="59.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.69921875" style="14" customWidth="1"/>
     <col min="11" max="11" width="15" style="14" customWidth="1"/>
-    <col min="12" max="12" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="56.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1320,7 +1408,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1348,7 +1436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1375,7 +1463,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1414,7 +1502,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1450,7 +1538,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1485,7 +1573,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1521,7 +1609,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1554,7 +1642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1587,7 +1675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1619,7 +1707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1651,7 +1739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1689,7 +1777,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1721,7 +1809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -1753,7 +1841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1785,7 +1873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -1817,7 +1905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1855,7 +1943,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1893,7 +1981,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -1921,7 +2009,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
@@ -1949,7 +2037,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
@@ -1977,7 +2065,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -2005,7 +2093,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
@@ -2033,7 +2121,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
@@ -2054,6 +2142,9 @@
       </c>
       <c r="G24" s="4" t="s">
         <v>31</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -2064,7 +2155,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -2092,175 +2183,164 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C26" s="7" t="s">
+    <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="G28" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="33">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="M29" s="32" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="33">
+        <v>2035</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+    </row>
+    <row r="31" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="M26" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="J28" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K28" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="J29" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K29" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>19</v>
@@ -2269,16 +2349,10 @@
         <v>69</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>10</v>
@@ -2287,13 +2361,13 @@
         <v>10</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>13</v>
       </c>
@@ -2301,7 +2375,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>206</v>
+        <v>44</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>19</v>
@@ -2310,7 +2384,10 @@
         <v>69</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>211</v>
+        <v>76</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="J32" s="13" t="s">
         <v>10</v>
@@ -2318,14 +2395,8 @@
       <c r="K32" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L32" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="M32" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>13</v>
       </c>
@@ -2333,7 +2404,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>203</v>
+        <v>45</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>19</v>
@@ -2342,7 +2413,13 @@
         <v>69</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>212</v>
+        <v>78</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="J33" s="13" t="s">
         <v>10</v>
@@ -2350,14 +2427,8 @@
       <c r="K33" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="M33" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
@@ -2365,7 +2436,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>205</v>
+        <v>107</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>19</v>
@@ -2374,7 +2445,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>213</v>
+        <v>111</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="J34" s="13" t="s">
         <v>10</v>
@@ -2382,14 +2459,8 @@
       <c r="K34" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L34" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>13</v>
       </c>
@@ -2397,7 +2468,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>19</v>
@@ -2406,7 +2477,13 @@
         <v>69</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>214</v>
+        <v>112</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="J35" s="13" t="s">
         <v>10</v>
@@ -2414,14 +2491,8 @@
       <c r="K35" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L35" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>13</v>
       </c>
@@ -2429,7 +2500,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>215</v>
+        <v>114</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>19</v>
@@ -2438,7 +2509,16 @@
         <v>69</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>211</v>
+        <v>115</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="J36" s="13" t="s">
         <v>10</v>
@@ -2447,13 +2527,13 @@
         <v>10</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>220</v>
+        <v>134</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>13</v>
       </c>
@@ -2461,7 +2541,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>19</v>
@@ -2470,7 +2550,7 @@
         <v>69</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J37" s="13" t="s">
         <v>10</v>
@@ -2479,13 +2559,13 @@
         <v>10</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="M37" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>13</v>
       </c>
@@ -2493,7 +2573,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>19</v>
@@ -2502,10 +2582,7 @@
         <v>69</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>31</v>
+        <v>212</v>
       </c>
       <c r="J38" s="13" t="s">
         <v>10</v>
@@ -2514,13 +2591,13 @@
         <v>10</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>13</v>
       </c>
@@ -2528,7 +2605,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>19</v>
@@ -2537,533 +2614,819 @@
         <v>69</v>
       </c>
       <c r="F39" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="J39" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L39" s="7" t="s">
+      <c r="J40" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K43" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L44" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="M39" s="7" t="s">
+      <c r="M44" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C40" s="15" t="s">
+    <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K45" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="G46" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C48" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" s="15" t="s">
+      <c r="D48" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F48" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H48" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I40" s="18" t="s">
+      <c r="I48" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="J40" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K40" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C41" s="15" t="s">
+      <c r="J48" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K48" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="15" t="s">
+      <c r="D49" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F49" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H49" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="I41" s="18" t="s">
+      <c r="I49" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="J41" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C42" s="15" t="s">
+      <c r="J49" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K49" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" s="15" t="s">
+      <c r="D50" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F50" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G50" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H50" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I42" s="18" t="s">
+      <c r="I50" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J42" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K42" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L42" s="15" t="s">
+      <c r="J50" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K50" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L50" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C43" s="15" t="s">
+    <row r="51" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" s="15" t="s">
+      <c r="D51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F51" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="H51" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I43" s="18" t="s">
+      <c r="I51" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="J43" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K43" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="15" t="s">
+      <c r="J51" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="15" t="s">
+      <c r="D52" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F52" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="H44" s="15" t="s">
+      <c r="H52" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I44" s="18" t="s">
+      <c r="I52" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="J44" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="15" t="s">
+      <c r="J52" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K52" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D45" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="15" t="s">
+      <c r="D53" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F53" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G53" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="H45" s="15" t="s">
+      <c r="H53" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I45" s="18"/>
-      <c r="J45" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K45" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L45" s="15" t="s">
+      <c r="I53" s="18"/>
+      <c r="J53" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K53" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L53" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="27" t="s">
+    <row r="54" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" s="25" t="s">
+      <c r="D54" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="F46" s="25" t="s">
+      <c r="F54" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="H46" s="27" t="s">
+      <c r="H54" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="I46" s="27" t="s">
+      <c r="I54" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="J46" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K46" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="27" t="s">
+      <c r="J54" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K54" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C55" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" s="25" t="s">
+      <c r="D55" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="F47" s="25" t="s">
+      <c r="F55" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H47" s="27" t="s">
+      <c r="H55" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="I47" s="27" t="s">
+      <c r="I55" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="J47" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K47" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="27" t="s">
+      <c r="J55" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K55" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="25" t="s">
+      <c r="D56" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="F48" s="25" t="s">
+      <c r="F56" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G48" s="27" t="s">
+      <c r="G56" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H48" s="27" t="s">
+      <c r="H56" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I48" s="27" t="s">
+      <c r="I56" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="J48" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K48" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L48" s="27" t="s">
+      <c r="J56" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K56" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L56" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="M48" s="27" t="s">
+      <c r="M56" s="27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C49" s="29" t="s">
+    <row r="57" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="D49" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="29" t="s">
+      <c r="D57" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="F57" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="H49" s="29" t="s">
+      <c r="H57" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="I49" s="29" t="s">
+      <c r="I57" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="J49" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K49" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C50" s="29" t="s">
+      <c r="J57" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K57" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D50" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E50" s="29" t="s">
+      <c r="D58" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="F58" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="H50" s="29" t="s">
+      <c r="H58" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="I50" s="29" t="s">
+      <c r="I58" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="J50" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K50" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="29" t="s">
+      <c r="J58" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K58" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="29" t="s">
+      <c r="D59" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F51" s="29" t="s">
+      <c r="F59" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="H51" s="29" t="s">
+      <c r="H59" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="I51" s="29" t="s">
+      <c r="I59" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="J51" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K51" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="L51" s="29" t="s">
+      <c r="J59" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K59" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L59" s="29" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B52" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="29" t="s">
+    <row r="60" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="D52" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="29" t="s">
+      <c r="D60" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F60" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="H52" s="29" t="s">
+      <c r="H60" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="I52" s="29" t="s">
+      <c r="I60" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="J52" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K52" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C53" s="29" t="s">
+      <c r="J60" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K60" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="D53" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E53" s="29" t="s">
+      <c r="D61" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="F61" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="H53" s="29" t="s">
+      <c r="H61" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="J53" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K53" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="29" t="s">
+      <c r="J61" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K61" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="D54" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" s="29" t="s">
+      <c r="D62" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="F54" s="29" t="s">
+      <c r="F62" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="G62" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H54" s="29" t="s">
+      <c r="H62" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="J54" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K54" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="L54" s="29" t="s">
+      <c r="J62" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L62" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="M54" s="29" t="s">
+      <c r="M62" s="29" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L59" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
     <hyperlink ref="I13" r:id="rId2" xr:uid="{088533EE-4DDB-4145-8A51-9A459A5B0EE7}"/>
-    <hyperlink ref="I40" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
+    <hyperlink ref="I48" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
updated noproject to 06
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atapase\OneDrive - Metropolitan Transportation Commission\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03FF70C-EC5B-48F2-A7C0-5843DE63EECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EC046F-9E71-47FA-90C7-32BD3EAA18BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="260">
   <si>
     <t>category</t>
   </si>
@@ -1394,7 +1394,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2568,9 +2568,6 @@
       <c r="F36" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G36" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="H36" s="7" t="s">
         <v>108</v>
       </c>

</xml_diff>

<commit_message>
updated with MBUF with transit runs
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atapase\OneDrive - Metropolitan Transportation Commission\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49C496E-989B-4FB1-B897-DA9BD8E27872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7BCF4A-39E0-4175-A827-507F8ECD8CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$64</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="264">
   <si>
     <t>category</t>
   </si>
@@ -816,6 +816,18 @@
   </si>
   <si>
     <t>F:\\Projects\\2035_TM160_NGFr2_NP06_Path2_01_LowCap</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_04_add2.9cT</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_04_add4.4cT</t>
+  </si>
+  <si>
+    <t>G:\\Projects\\2035_TM160_NGF_r2_NoProject_04_add2.9cT</t>
+  </si>
+  <si>
+    <t>V:\\Projects\\2035_TM160_NGF_r2_NoProject_04_add4.4cT</t>
   </si>
 </sst>
 </file>
@@ -1390,11 +1402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2340,9 +2352,7 @@
       <c r="F29" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="G29" s="35" t="s">
-        <v>31</v>
-      </c>
+      <c r="G29" s="35"/>
       <c r="H29" s="32" t="s">
         <v>224</v>
       </c>
@@ -2377,9 +2387,7 @@
       <c r="F30" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="G30" s="35" t="s">
-        <v>31</v>
-      </c>
+      <c r="G30" s="35"/>
       <c r="J30" s="34"/>
       <c r="K30" s="34"/>
       <c r="L30" s="32" t="s">
@@ -2988,9 +2996,7 @@
       <c r="F48" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="G48" s="36" t="s">
-        <v>31</v>
-      </c>
+      <c r="G48" s="36"/>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="7" t="s">
@@ -3019,9 +3025,7 @@
       <c r="F49" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="G49" s="36" t="s">
-        <v>31</v>
-      </c>
+      <c r="G49" s="36"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
       <c r="L49" s="7" t="s">
@@ -3050,9 +3054,7 @@
       <c r="F50" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="G50" s="36" t="s">
-        <v>31</v>
-      </c>
+      <c r="G50" s="36"/>
       <c r="J50" s="13"/>
       <c r="K50" s="13"/>
       <c r="L50" s="7" t="s">
@@ -3062,68 +3064,66 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I51" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J51" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K51" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B52" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I52" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="J52" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K52" s="17" t="s">
-        <v>10</v>
+    <row r="51" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="G51" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="G52" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -3134,7 +3134,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>19</v>
@@ -3143,25 +3143,19 @@
         <v>91</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="I53" s="18" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="J53" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K53" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="L53" s="15" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -3172,7 +3166,7 @@
         <v>2035</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>19</v>
@@ -3181,13 +3175,13 @@
         <v>91</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="I54" s="18" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J54" s="17" t="s">
         <v>10</v>
@@ -3204,7 +3198,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>19</v>
@@ -3213,19 +3207,25 @@
         <v>91</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="H55" s="15" t="s">
         <v>119</v>
       </c>
       <c r="I55" s="18" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="J55" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K55" s="17" t="s">
         <v>10</v>
+      </c>
+      <c r="L55" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -3236,7 +3236,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>19</v>
@@ -3245,87 +3245,87 @@
         <v>91</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H56" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I56" s="18"/>
+      <c r="I56" s="18" t="s">
+        <v>120</v>
+      </c>
       <c r="J56" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K56" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L56" s="15" t="s">
+    </row>
+    <row r="57" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I57" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J57" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K57" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I58" s="18"/>
+      <c r="J58" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K58" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L58" s="15" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F57" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H57" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="I57" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J57" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K57" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C58" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E58" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F58" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="H58" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="I58" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="J58" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K58" s="28" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
@@ -3336,7 +3336,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>19</v>
@@ -3345,92 +3345,92 @@
         <v>92</v>
       </c>
       <c r="F59" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H59" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="I59" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="J59" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K59" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F60" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H60" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I60" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J60" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K60" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F61" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G59" s="27" t="s">
+      <c r="G61" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H59" s="27" t="s">
+      <c r="H61" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I59" s="27" t="s">
+      <c r="I61" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="J59" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K59" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L59" s="27" t="s">
+      <c r="J61" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K61" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L61" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="M59" s="27" t="s">
+      <c r="M61" s="27" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E60" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F60" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H60" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="I60" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="J60" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K60" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E61" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F61" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="H61" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I61" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="J61" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K61" s="31" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
@@ -3441,7 +3441,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="D62" s="29" t="s">
         <v>19</v>
@@ -3450,22 +3450,19 @@
         <v>117</v>
       </c>
       <c r="F62" s="29" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H62" s="29" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="I62" s="29" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J62" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K62" s="31" t="s">
         <v>10</v>
-      </c>
-      <c r="L62" s="29" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
@@ -3476,7 +3473,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="D63" s="29" t="s">
         <v>19</v>
@@ -3485,13 +3482,13 @@
         <v>117</v>
       </c>
       <c r="F63" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H63" s="29" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="I63" s="29" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="J63" s="31" t="s">
         <v>10</v>
@@ -3508,7 +3505,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D64" s="29" t="s">
         <v>19</v>
@@ -3517,16 +3514,22 @@
         <v>117</v>
       </c>
       <c r="F64" s="29" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="H64" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="I64" s="29" t="s">
+        <v>128</v>
       </c>
       <c r="J64" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K64" s="31" t="s">
         <v>10</v>
+      </c>
+      <c r="L64" s="29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
@@ -3537,7 +3540,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D65" s="29" t="s">
         <v>19</v>
@@ -3546,34 +3549,95 @@
         <v>117</v>
       </c>
       <c r="F65" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G65" s="29" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="H65" s="29" t="s">
         <v>143</v>
       </c>
+      <c r="I65" s="29" t="s">
+        <v>144</v>
+      </c>
       <c r="J65" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K65" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L65" s="29" t="s">
+    </row>
+    <row r="66" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C66" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H66" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J66" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K66" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G67" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H67" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J67" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K67" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L67" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="M65" s="29" t="s">
+      <c r="M67" s="29" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L62" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
     <hyperlink ref="I13" r:id="rId2" xr:uid="{088533EE-4DDB-4145-8A51-9A459A5B0EE7}"/>
-    <hyperlink ref="I51" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
+    <hyperlink ref="I53" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
added two "post tollclass=0 bug fix" runs to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atapase\OneDrive - Metropolitan Transportation Commission\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E7A9D4-2167-4F81-B6AA-992AB4D139D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5477CED-FD67-4ECC-A4A7-A437951F1097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="265">
   <si>
     <t>category</t>
   </si>
@@ -716,9 +716,6 @@
     <t>https://app.asana.com/0/0/1207994963427970/f</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>2035_TM160_NGF_r2_NoProject_05</t>
   </si>
   <si>
@@ -740,15 +737,6 @@
     <t>https://app.asana.com/0/0/1207994963427971/f</t>
   </si>
   <si>
-    <t>to be started</t>
-  </si>
-  <si>
-    <t>2035_TM160_NGF_r2_NoProject_05_add4.4c</t>
-  </si>
-  <si>
-    <t>NP run - no EL, AOC+4.4c</t>
-  </si>
-  <si>
     <t>NP run - no EL, MBUF at 4.4c</t>
   </si>
   <si>
@@ -828,6 +816,21 @@
   </si>
   <si>
     <t>V:\\Projects\\2035_TM160_NGF_r2_NoProject_04_add4.4cT</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP06_Path2_02</t>
+  </si>
+  <si>
+    <t>being debugged</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_06_link4.4mb2</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1208050271845385/f</t>
+  </si>
+  <si>
+    <t>P2- MBUF post tollclass=0 bug fix, at 7.5c</t>
   </si>
 </sst>
 </file>
@@ -1402,29 +1405,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.3984375" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.140625" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
-    <col min="9" max="9" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" customWidth="1"/>
+    <col min="5" max="5" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.09765625" customWidth="1"/>
+    <col min="8" max="8" width="47.3984375" customWidth="1"/>
+    <col min="9" max="9" width="59.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.69921875" style="14" customWidth="1"/>
     <col min="11" max="11" width="15" style="14" customWidth="1"/>
-    <col min="12" max="12" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="56.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1595,7 +1598,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1666,7 +1669,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1699,7 +1702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1732,7 +1735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1834,7 +1837,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1930,7 +1933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -1962,7 +1965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>19</v>
@@ -2257,25 +2260,25 @@
         <v>28</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G26" s="37"/>
       <c r="H26" s="4" t="s">
         <v>224</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>19</v>
@@ -2292,19 +2295,19 @@
         <v>28</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G27" s="37"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>13</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>19</v>
@@ -2321,13 +2324,13 @@
         <v>28</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G28" s="37"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
         <v>13</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>2035</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>19</v>
@@ -2344,7 +2347,7 @@
         <v>223</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G29" s="35"/>
       <c r="H29" s="32" t="s">
@@ -2356,13 +2359,13 @@
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
       <c r="L29" s="32" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="M29" s="32" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="s">
         <v>13</v>
       </c>
@@ -2370,7 +2373,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>19</v>
@@ -2379,62 +2382,58 @@
         <v>223</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G30" s="35"/>
       <c r="J30" s="34"/>
       <c r="K30" s="34"/>
       <c r="L30" s="32" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="M30" s="32" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C31" s="7" t="s">
+    <row r="31" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="33">
+        <v>2035</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+    </row>
+    <row r="32" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K31" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L31" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="M31" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>19</v>
@@ -2443,10 +2442,10 @@
         <v>69</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J32" s="13" t="s">
         <v>10</v>
@@ -2454,8 +2453,14 @@
       <c r="K32" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L32" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>13</v>
       </c>
@@ -2463,7 +2468,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>19</v>
@@ -2472,13 +2477,10 @@
         <v>69</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J33" s="13" t="s">
         <v>10</v>
@@ -2487,7 +2489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
@@ -2495,7 +2497,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>19</v>
@@ -2504,13 +2506,13 @@
         <v>69</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="J34" s="13" t="s">
         <v>10</v>
@@ -2519,7 +2521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>13</v>
       </c>
@@ -2527,7 +2529,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>19</v>
@@ -2536,13 +2538,13 @@
         <v>69</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J35" s="13" t="s">
         <v>10</v>
@@ -2551,7 +2553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>13</v>
       </c>
@@ -2559,7 +2561,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>19</v>
@@ -2568,16 +2570,13 @@
         <v>69</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J36" s="13" t="s">
         <v>10</v>
@@ -2585,14 +2584,8 @@
       <c r="K36" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L36" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="M36" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>13</v>
       </c>
@@ -2600,7 +2593,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>206</v>
+        <v>114</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>19</v>
@@ -2609,7 +2602,16 @@
         <v>69</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>211</v>
+        <v>115</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="J37" s="13" t="s">
         <v>10</v>
@@ -2618,13 +2620,13 @@
         <v>10</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="M37" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>13</v>
       </c>
@@ -2632,7 +2634,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>19</v>
@@ -2641,7 +2643,7 @@
         <v>69</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J38" s="13" t="s">
         <v>10</v>
@@ -2650,13 +2652,13 @@
         <v>10</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>13</v>
       </c>
@@ -2664,7 +2666,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>19</v>
@@ -2673,7 +2675,7 @@
         <v>69</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J39" s="13" t="s">
         <v>10</v>
@@ -2682,13 +2684,13 @@
         <v>10</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M39" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>13</v>
       </c>
@@ -2696,7 +2698,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>19</v>
@@ -2705,7 +2707,7 @@
         <v>69</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J40" s="13" t="s">
         <v>10</v>
@@ -2714,13 +2716,13 @@
         <v>10</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>13</v>
       </c>
@@ -2728,7 +2730,7 @@
         <v>2035</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>19</v>
@@ -2737,7 +2739,7 @@
         <v>69</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="J41" s="13" t="s">
         <v>10</v>
@@ -2746,13 +2748,13 @@
         <v>10</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>13</v>
       </c>
@@ -2760,7 +2762,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>19</v>
@@ -2769,7 +2771,7 @@
         <v>69</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J42" s="13" t="s">
         <v>10</v>
@@ -2778,13 +2780,13 @@
         <v>10</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>13</v>
       </c>
@@ -2792,7 +2794,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>19</v>
@@ -2801,7 +2803,7 @@
         <v>69</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J43" s="13" t="s">
         <v>10</v>
@@ -2810,13 +2812,13 @@
         <v>10</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>13</v>
       </c>
@@ -2824,7 +2826,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>19</v>
@@ -2833,7 +2835,7 @@
         <v>69</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J44" s="13" t="s">
         <v>10</v>
@@ -2842,13 +2844,13 @@
         <v>10</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>13</v>
       </c>
@@ -2856,7 +2858,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>19</v>
@@ -2865,16 +2867,7 @@
         <v>69</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="G45" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="J45" s="13" t="s">
         <v>10</v>
@@ -2889,7 +2882,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>13</v>
       </c>
@@ -2897,7 +2890,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>19</v>
@@ -2906,31 +2899,21 @@
         <v>69</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G46" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="J46" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K46" s="13" t="s">
-        <v>10</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
       <c r="L46" s="7" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="M46" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
@@ -2938,7 +2921,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>19</v>
@@ -2947,31 +2930,21 @@
         <v>69</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="G47" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="J47" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K47" s="13" t="s">
-        <v>10</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
       <c r="L47" s="7" t="s">
-        <v>222</v>
+        <v>259</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>13</v>
       </c>
@@ -2979,7 +2952,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>19</v>
@@ -2988,19 +2961,29 @@
         <v>69</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="G48" s="36"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
+      <c r="H48" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="J48" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="L48" s="7" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>13</v>
       </c>
@@ -3008,7 +2991,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>19</v>
@@ -3017,19 +3000,29 @@
         <v>69</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="G49" s="36"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
+      <c r="H49" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="J49" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K49" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="L49" s="7" t="s">
-        <v>252</v>
+        <v>222</v>
       </c>
       <c r="M49" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>13</v>
       </c>
@@ -3037,7 +3030,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>19</v>
@@ -3046,19 +3039,19 @@
         <v>69</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G50" s="36"/>
       <c r="J50" s="13"/>
       <c r="K50" s="13"/>
       <c r="L50" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>13</v>
       </c>
@@ -3066,7 +3059,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>19</v>
@@ -3075,21 +3068,19 @@
         <v>69</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="G51" s="36" t="s">
-        <v>31</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="G51" s="36"/>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
       <c r="L51" s="7" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="M51" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>13</v>
       </c>
@@ -3097,7 +3088,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>19</v>
@@ -3106,61 +3097,58 @@
         <v>69</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="G52" s="36" t="s">
-        <v>31</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="G52" s="36"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="G53" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I53" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="M52" s="7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C53" s="15" t="s">
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+    </row>
+    <row r="54" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H53" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I53" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J53" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K53" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>19</v>
@@ -3169,13 +3157,13 @@
         <v>91</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I54" s="18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J54" s="17" t="s">
         <v>10</v>
@@ -3184,7 +3172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
         <v>13</v>
       </c>
@@ -3192,7 +3180,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>122</v>
+        <v>84</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>19</v>
@@ -3201,16 +3189,13 @@
         <v>91</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="I55" s="18" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="J55" s="17" t="s">
         <v>10</v>
@@ -3218,11 +3203,8 @@
       <c r="K55" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L55" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
         <v>13</v>
       </c>
@@ -3230,7 +3212,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>19</v>
@@ -3239,13 +3221,16 @@
         <v>91</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>148</v>
+        <v>126</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="H56" s="15" t="s">
         <v>119</v>
       </c>
       <c r="I56" s="18" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="J56" s="17" t="s">
         <v>10</v>
@@ -3253,8 +3238,11 @@
       <c r="K56" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L56" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
         <v>13</v>
       </c>
@@ -3262,7 +3250,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>19</v>
@@ -3271,7 +3259,7 @@
         <v>91</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H57" s="15" t="s">
         <v>119</v>
@@ -3286,7 +3274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
         <v>13</v>
       </c>
@@ -3294,7 +3282,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>19</v>
@@ -3303,66 +3291,66 @@
         <v>91</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H58" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I58" s="18"/>
+      <c r="I58" s="18" t="s">
+        <v>120</v>
+      </c>
       <c r="J58" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K58" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L58" s="15" t="s">
+    </row>
+    <row r="59" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I59" s="18"/>
+      <c r="J59" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K59" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L59" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B59" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C59" s="27" t="s">
+    <row r="60" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="27" t="s">
         <v>89</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E59" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F59" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H59" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="I59" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J59" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K59" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="27" t="s">
-        <v>88</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>19</v>
@@ -3371,13 +3359,13 @@
         <v>92</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H60" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I60" s="27" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J60" s="28" t="s">
         <v>10</v>
@@ -3386,7 +3374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
         <v>13</v>
       </c>
@@ -3394,7 +3382,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>19</v>
@@ -3403,71 +3391,71 @@
         <v>92</v>
       </c>
       <c r="F61" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H61" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I61" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J61" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K61" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F62" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G61" s="27" t="s">
+      <c r="G62" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H61" s="27" t="s">
+      <c r="H62" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I61" s="27" t="s">
+      <c r="I62" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="J61" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K61" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L61" s="27" t="s">
+      <c r="J62" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L62" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="M61" s="27" t="s">
+      <c r="M62" s="27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C62" s="29" t="s">
+    <row r="63" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="29" t="s">
         <v>99</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F62" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H62" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="I62" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="J62" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K62" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C63" s="29" t="s">
-        <v>100</v>
       </c>
       <c r="D63" s="29" t="s">
         <v>19</v>
@@ -3476,13 +3464,13 @@
         <v>117</v>
       </c>
       <c r="F63" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H63" s="29" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I63" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J63" s="31" t="s">
         <v>10</v>
@@ -3491,7 +3479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="29" t="s">
         <v>13</v>
       </c>
@@ -3499,7 +3487,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D64" s="29" t="s">
         <v>19</v>
@@ -3508,13 +3496,13 @@
         <v>117</v>
       </c>
       <c r="F64" s="29" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="H64" s="29" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="I64" s="29" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="J64" s="31" t="s">
         <v>10</v>
@@ -3522,11 +3510,8 @@
       <c r="K64" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L64" s="29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="29" t="s">
         <v>13</v>
       </c>
@@ -3534,7 +3519,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="D65" s="29" t="s">
         <v>19</v>
@@ -3543,13 +3528,13 @@
         <v>117</v>
       </c>
       <c r="F65" s="29" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I65" s="29" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="J65" s="31" t="s">
         <v>10</v>
@@ -3557,8 +3542,11 @@
       <c r="K65" s="31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L65" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="29" t="s">
         <v>13</v>
       </c>
@@ -3566,7 +3554,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D66" s="29" t="s">
         <v>19</v>
@@ -3575,11 +3563,14 @@
         <v>117</v>
       </c>
       <c r="F66" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H66" s="29" t="s">
         <v>143</v>
       </c>
+      <c r="I66" s="29" t="s">
+        <v>144</v>
+      </c>
       <c r="J66" s="31" t="s">
         <v>10</v>
       </c>
@@ -3587,7 +3578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="29" t="s">
         <v>13</v>
       </c>
@@ -3595,7 +3586,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D67" s="29" t="s">
         <v>19</v>
@@ -3604,10 +3595,7 @@
         <v>117</v>
       </c>
       <c r="F67" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G67" s="29" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="H67" s="29" t="s">
         <v>143</v>
@@ -3618,20 +3606,52 @@
       <c r="K67" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L67" s="29" t="s">
+    </row>
+    <row r="68" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C68" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G68" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H68" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J68" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K68" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L68" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="M67" s="29" t="s">
+      <c r="M68" s="29" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L65" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
     <hyperlink ref="I13" r:id="rId2" xr:uid="{088533EE-4DDB-4145-8A51-9A459A5B0EE7}"/>
-    <hyperlink ref="I53" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
+    <hyperlink ref="I54" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
added two AOC-based MBUF runs (for toll cap post-processing) to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5477CED-FD67-4ECC-A4A7-A437951F1097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194491E1-8E85-43F1-A5CA-83B27A88A8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="271">
   <si>
     <t>category</t>
   </si>
@@ -831,6 +831,24 @@
   </si>
   <si>
     <t>P2- MBUF post tollclass=0 bug fix, at 7.5c</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_06_add2.9cT</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_06_add4.4cT</t>
+  </si>
+  <si>
+    <t>aoc based mbuf at 5c, no cap, network with more transit</t>
+  </si>
+  <si>
+    <t>aoc based mbuf at 7.5c, no cap, network with more transit</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NGFround2_P2_01</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1208050271846456/f</t>
   </si>
 </sst>
 </file>
@@ -1405,11 +1423,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD51"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2904,6 +2922,9 @@
       <c r="G46" s="36" t="s">
         <v>31</v>
       </c>
+      <c r="H46" s="7" t="s">
+        <v>269</v>
+      </c>
       <c r="J46" s="13"/>
       <c r="K46" s="13"/>
       <c r="L46" s="7" t="s">
@@ -2934,6 +2955,9 @@
       </c>
       <c r="G47" s="36" t="s">
         <v>31</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>269</v>
       </c>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
@@ -3140,69 +3164,67 @@
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
     </row>
-    <row r="54" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I54" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J54" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K54" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I55" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="J55" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K55" s="17" t="s">
-        <v>10</v>
-      </c>
+    <row r="54" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G54" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+    </row>
+    <row r="55" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="G55" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
     </row>
     <row r="56" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
@@ -3212,7 +3234,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>19</v>
@@ -3221,25 +3243,19 @@
         <v>91</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="I56" s="18" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="J56" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K56" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="L56" s="15" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3250,7 +3266,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>19</v>
@@ -3259,13 +3275,13 @@
         <v>91</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J57" s="17" t="s">
         <v>10</v>
@@ -3282,7 +3298,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>19</v>
@@ -3291,19 +3307,25 @@
         <v>91</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="H58" s="15" t="s">
         <v>119</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="J58" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K58" s="17" t="s">
         <v>10</v>
+      </c>
+      <c r="L58" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3314,7 +3336,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>19</v>
@@ -3323,87 +3345,87 @@
         <v>91</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H59" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I59" s="18"/>
+      <c r="I59" s="18" t="s">
+        <v>120</v>
+      </c>
       <c r="J59" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K59" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L59" s="15" t="s">
+    </row>
+    <row r="60" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I60" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J60" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K60" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G61" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I61" s="18"/>
+      <c r="J61" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K61" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L61" s="15" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E60" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F60" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H60" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="I60" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J60" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K60" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C61" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D61" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E61" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F61" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="H61" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="I61" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="J61" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K61" s="28" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
@@ -3414,7 +3436,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>19</v>
@@ -3423,92 +3445,92 @@
         <v>92</v>
       </c>
       <c r="F62" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H62" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="I62" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="J62" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F63" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H63" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I63" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J63" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K63" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C64" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F64" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G62" s="27" t="s">
+      <c r="G64" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H62" s="27" t="s">
+      <c r="H64" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I62" s="27" t="s">
+      <c r="I64" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="J62" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K62" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L62" s="27" t="s">
+      <c r="J64" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K64" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L64" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="M62" s="27" t="s">
+      <c r="M64" s="27" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C63" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F63" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H63" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="I63" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="J63" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K63" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C64" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D64" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E64" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F64" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="H64" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I64" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="J64" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K64" s="31" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -3519,7 +3541,7 @@
         <v>2035</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="D65" s="29" t="s">
         <v>19</v>
@@ -3528,22 +3550,19 @@
         <v>117</v>
       </c>
       <c r="F65" s="29" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="I65" s="29" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J65" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K65" s="31" t="s">
         <v>10</v>
-      </c>
-      <c r="L65" s="29" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -3554,7 +3573,7 @@
         <v>2035</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="D66" s="29" t="s">
         <v>19</v>
@@ -3563,13 +3582,13 @@
         <v>117</v>
       </c>
       <c r="F66" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H66" s="29" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="I66" s="29" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="J66" s="31" t="s">
         <v>10</v>
@@ -3586,7 +3605,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D67" s="29" t="s">
         <v>19</v>
@@ -3595,16 +3614,22 @@
         <v>117</v>
       </c>
       <c r="F67" s="29" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="H67" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="I67" s="29" t="s">
+        <v>128</v>
       </c>
       <c r="J67" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K67" s="31" t="s">
         <v>10</v>
+      </c>
+      <c r="L67" s="29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -3615,7 +3640,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D68" s="29" t="s">
         <v>19</v>
@@ -3624,34 +3649,95 @@
         <v>117</v>
       </c>
       <c r="F68" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G68" s="29" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>143</v>
       </c>
+      <c r="I68" s="29" t="s">
+        <v>144</v>
+      </c>
       <c r="J68" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K68" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L68" s="29" t="s">
+    </row>
+    <row r="69" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H69" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J69" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K69" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C70" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F70" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G70" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H70" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J70" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K70" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L70" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="M68" s="29" t="s">
+      <c r="M70" s="29" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L65" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
     <hyperlink ref="I13" r:id="rId2" xr:uid="{088533EE-4DDB-4145-8A51-9A459A5B0EE7}"/>
-    <hyperlink ref="I54" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
+    <hyperlink ref="I56" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
add NoProject_07 and an alternative P1_12 to the model run log
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194491E1-8E85-43F1-A5CA-83B27A88A8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F874A005-F7AC-4084-B809-515DC6978F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="280">
   <si>
     <t>category</t>
   </si>
@@ -791,9 +791,6 @@
     <t>xxz</t>
   </si>
   <si>
-    <t>xxx</t>
-  </si>
-  <si>
     <t>2035_TM160_NGFr2_NP06_Path2_01</t>
   </si>
   <si>
@@ -849,6 +846,36 @@
   </si>
   <si>
     <t>https://app.asana.com/0/1203644633064654/1208050271846456/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_07</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1208068566505509/f</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>same trn hes as NoProject_06 but with EL on</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1208025230758033/f</t>
+  </si>
+  <si>
+    <t>updated trn hes (less trn hes than NoProject_04 and 05); no EL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked-based MBUF test after the tollclass=0 bug fix </t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP04_Path1_12_highTrnHes</t>
+  </si>
+  <si>
+    <t>P1 - 30c/10c - no local road spd limit red (but use old i.e. higher trn hes)</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1208068566505517/f</t>
   </si>
 </sst>
 </file>
@@ -1423,11 +1450,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2241,7 +2268,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>179</v>
+        <v>277</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>19</v>
@@ -2250,16 +2277,19 @@
         <v>28</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>184</v>
+        <v>278</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
-      <c r="L25" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>193</v>
-      </c>
     </row>
     <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -2269,7 +2299,7 @@
         <v>2035</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>243</v>
+        <v>179</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>19</v>
@@ -2278,22 +2308,15 @@
         <v>28</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="G26" s="37"/>
-      <c r="H26" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="4" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2304,7 +2327,7 @@
         <v>2035</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>19</v>
@@ -2313,16 +2336,22 @@
         <v>28</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="G27" s="37"/>
+      <c r="H27" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>228</v>
+      </c>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2333,7 +2362,7 @@
         <v>2035</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>19</v>
@@ -2342,46 +2371,40 @@
         <v>28</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="G28" s="37"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
-    </row>
-    <row r="29" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="33">
-        <v>2035</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>252</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>234</v>
-      </c>
-      <c r="G29" s="35"/>
-      <c r="H29" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="I29" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="32" t="s">
-        <v>254</v>
-      </c>
-      <c r="M29" s="32" t="s">
-        <v>189</v>
-      </c>
+      <c r="L28" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2035</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G29" s="37"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
     </row>
     <row r="30" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="s">
@@ -2391,7 +2414,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>19</v>
@@ -2400,16 +2423,22 @@
         <v>223</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G30" s="35"/>
+      <c r="H30" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>225</v>
+      </c>
       <c r="J30" s="34"/>
       <c r="K30" s="34"/>
       <c r="L30" s="32" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M30" s="32" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -2420,7 +2449,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D31" s="32" t="s">
         <v>19</v>
@@ -2429,54 +2458,48 @@
         <v>223</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="G31" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="I31" s="32" t="s">
-        <v>263</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="G31" s="35"/>
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
-    </row>
-    <row r="32" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="8">
-        <v>2035</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L32" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="M32" s="7" t="s">
-        <v>189</v>
-      </c>
+      <c r="L31" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="M31" s="32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="33">
+        <v>2035</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
     </row>
     <row r="33" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
@@ -2486,7 +2509,7 @@
         <v>2035</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>19</v>
@@ -2495,16 +2518,22 @@
         <v>69</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J33" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K33" s="13" t="s">
         <v>10</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2515,7 +2544,7 @@
         <v>2035</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>19</v>
@@ -2524,13 +2553,10 @@
         <v>69</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J34" s="13" t="s">
         <v>10</v>
@@ -2547,7 +2573,7 @@
         <v>2035</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>19</v>
@@ -2556,13 +2582,13 @@
         <v>69</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="J35" s="13" t="s">
         <v>10</v>
@@ -2579,7 +2605,7 @@
         <v>2035</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>19</v>
@@ -2588,13 +2614,13 @@
         <v>69</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J36" s="13" t="s">
         <v>10</v>
@@ -2611,7 +2637,7 @@
         <v>2035</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>19</v>
@@ -2620,28 +2646,19 @@
         <v>69</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J37" s="13" t="s">
         <v>10</v>
       </c>
       <c r="K37" s="13" t="s">
         <v>10</v>
-      </c>
-      <c r="L37" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="M37" s="7" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2652,7 +2669,7 @@
         <v>2035</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>206</v>
+        <v>114</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>19</v>
@@ -2661,7 +2678,16 @@
         <v>69</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>211</v>
+        <v>115</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="J38" s="13" t="s">
         <v>10</v>
@@ -2670,10 +2696,10 @@
         <v>10</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2684,7 +2710,7 @@
         <v>2035</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>19</v>
@@ -2693,7 +2719,7 @@
         <v>69</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J39" s="13" t="s">
         <v>10</v>
@@ -2702,10 +2728,10 @@
         <v>10</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M39" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2716,7 +2742,7 @@
         <v>2035</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>19</v>
@@ -2725,7 +2751,7 @@
         <v>69</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J40" s="13" t="s">
         <v>10</v>
@@ -2734,10 +2760,10 @@
         <v>10</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2748,7 +2774,7 @@
         <v>2035</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>19</v>
@@ -2757,7 +2783,7 @@
         <v>69</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J41" s="13" t="s">
         <v>10</v>
@@ -2766,10 +2792,10 @@
         <v>10</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2780,7 +2806,7 @@
         <v>2035</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>19</v>
@@ -2789,7 +2815,7 @@
         <v>69</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="J42" s="13" t="s">
         <v>10</v>
@@ -2798,10 +2824,10 @@
         <v>10</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2812,7 +2838,7 @@
         <v>2035</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>19</v>
@@ -2821,7 +2847,7 @@
         <v>69</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J43" s="13" t="s">
         <v>10</v>
@@ -2830,10 +2856,10 @@
         <v>10</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2844,7 +2870,7 @@
         <v>2035</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>19</v>
@@ -2853,7 +2879,7 @@
         <v>69</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J44" s="13" t="s">
         <v>10</v>
@@ -2862,10 +2888,10 @@
         <v>10</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2876,7 +2902,7 @@
         <v>2035</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>19</v>
@@ -2885,7 +2911,7 @@
         <v>69</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J45" s="13" t="s">
         <v>10</v>
@@ -2894,10 +2920,10 @@
         <v>10</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M45" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2908,7 +2934,7 @@
         <v>2035</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>19</v>
@@ -2917,21 +2943,19 @@
         <v>69</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G46" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
+        <v>214</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="L46" s="7" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="M46" s="7" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2942,7 +2966,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>19</v>
@@ -2957,15 +2981,15 @@
         <v>31</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
       <c r="L47" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>240</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2976,7 +3000,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>19</v>
@@ -2985,26 +3009,21 @@
         <v>69</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="G48" s="36"/>
+        <v>250</v>
+      </c>
+      <c r="G48" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="H48" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I48" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="J48" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K48" s="13" t="s">
-        <v>10</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
       <c r="L48" s="7" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>193</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3015,7 +3034,7 @@
         <v>2035</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>19</v>
@@ -3024,14 +3043,14 @@
         <v>69</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G49" s="36"/>
       <c r="H49" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J49" s="13" t="s">
         <v>10</v>
@@ -3054,7 +3073,7 @@
         <v>2035</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>19</v>
@@ -3063,16 +3082,26 @@
         <v>69</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="G50" s="36"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
+      <c r="H50" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="J50" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="L50" s="7" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>240</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3083,7 +3112,7 @@
         <v>2035</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>19</v>
@@ -3092,16 +3121,24 @@
         <v>69</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="G51" s="36"/>
+        <v>275</v>
+      </c>
+      <c r="G51" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>274</v>
+      </c>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
       <c r="L51" s="7" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="M51" s="7" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3112,7 +3149,7 @@
         <v>2035</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>19</v>
@@ -3121,16 +3158,16 @@
         <v>69</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G52" s="36"/>
       <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="7" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="M52" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3141,7 +3178,7 @@
         <v>2035</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>19</v>
@@ -3152,17 +3189,15 @@
       <c r="F53" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="G53" s="36" t="s">
-        <v>261</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>263</v>
-      </c>
+      <c r="G53" s="36"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
+      <c r="L53" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="54" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
@@ -3172,7 +3207,7 @@
         <v>2035</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>19</v>
@@ -3181,16 +3216,16 @@
         <v>69</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="G54" s="36" t="s">
-        <v>31</v>
+        <v>260</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>269</v>
+        <v>108</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
@@ -3203,7 +3238,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>19</v>
@@ -3212,82 +3247,86 @@
         <v>69</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G55" s="36" t="s">
         <v>31</v>
       </c>
       <c r="H55" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I55" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="I55" s="7" t="s">
-        <v>270</v>
       </c>
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
     </row>
-    <row r="56" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F56" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H56" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I56" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K56" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F57" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H57" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I57" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="J57" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K57" s="17" t="s">
-        <v>10</v>
+    <row r="56" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G56" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+    </row>
+    <row r="57" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="G57" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3298,7 +3337,7 @@
         <v>2035</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>19</v>
@@ -3307,25 +3346,19 @@
         <v>91</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="J58" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K58" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="L58" s="15" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3336,7 +3369,7 @@
         <v>2035</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>19</v>
@@ -3345,13 +3378,13 @@
         <v>91</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="I59" s="18" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J59" s="17" t="s">
         <v>10</v>
@@ -3368,7 +3401,7 @@
         <v>2035</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>19</v>
@@ -3377,19 +3410,25 @@
         <v>91</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="H60" s="15" t="s">
         <v>119</v>
       </c>
       <c r="I60" s="18" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="J60" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K60" s="17" t="s">
         <v>10</v>
+      </c>
+      <c r="L60" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3400,7 +3439,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>19</v>
@@ -3409,87 +3448,87 @@
         <v>91</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G61" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H61" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I61" s="18"/>
+      <c r="I61" s="18" t="s">
+        <v>120</v>
+      </c>
       <c r="J61" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K61" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L61" s="15" t="s">
+    </row>
+    <row r="62" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I62" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J62" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I63" s="18"/>
+      <c r="J63" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K63" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L63" s="15" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C62" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E62" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F62" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H62" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="I62" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J62" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K62" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C63" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D63" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="F63" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="H63" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="I63" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="J63" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K63" s="28" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
@@ -3500,7 +3539,7 @@
         <v>2035</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>19</v>
@@ -3509,92 +3548,92 @@
         <v>92</v>
       </c>
       <c r="F64" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H64" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="I64" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="J64" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K64" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F65" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H65" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I65" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J65" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K65" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C66" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G64" s="27" t="s">
+      <c r="G66" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H64" s="27" t="s">
+      <c r="H66" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I64" s="27" t="s">
+      <c r="I66" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="J64" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K64" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L64" s="27" t="s">
+      <c r="J66" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K66" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L66" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="M64" s="27" t="s">
+      <c r="M66" s="27" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B65" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C65" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D65" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E65" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F65" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H65" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="I65" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="J65" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K65" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C66" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E66" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F66" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="H66" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I66" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="J66" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K66" s="31" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -3605,7 +3644,7 @@
         <v>2035</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="D67" s="29" t="s">
         <v>19</v>
@@ -3614,22 +3653,19 @@
         <v>117</v>
       </c>
       <c r="F67" s="29" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H67" s="29" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="I67" s="29" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J67" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K67" s="31" t="s">
         <v>10</v>
-      </c>
-      <c r="L67" s="29" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -3640,7 +3676,7 @@
         <v>2035</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="D68" s="29" t="s">
         <v>19</v>
@@ -3649,13 +3685,13 @@
         <v>117</v>
       </c>
       <c r="F68" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H68" s="29" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="I68" s="29" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="J68" s="31" t="s">
         <v>10</v>
@@ -3672,7 +3708,7 @@
         <v>2035</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D69" s="29" t="s">
         <v>19</v>
@@ -3681,16 +3717,22 @@
         <v>117</v>
       </c>
       <c r="F69" s="29" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="H69" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="I69" s="29" t="s">
+        <v>128</v>
       </c>
       <c r="J69" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K69" s="31" t="s">
         <v>10</v>
+      </c>
+      <c r="L69" s="29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -3701,7 +3743,7 @@
         <v>2035</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D70" s="29" t="s">
         <v>19</v>
@@ -3710,34 +3752,95 @@
         <v>117</v>
       </c>
       <c r="F70" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G70" s="29" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="H70" s="29" t="s">
         <v>143</v>
       </c>
+      <c r="I70" s="29" t="s">
+        <v>144</v>
+      </c>
       <c r="J70" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K70" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L70" s="29" t="s">
+    </row>
+    <row r="71" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C71" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F71" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H71" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J71" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K71" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C72" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F72" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G72" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H72" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J72" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K72" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L72" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="M70" s="29" t="s">
+      <c r="M72" s="29" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
     <hyperlink ref="I13" r:id="rId2" xr:uid="{088533EE-4DDB-4145-8A51-9A459A5B0EE7}"/>
-    <hyperlink ref="I56" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
+    <hyperlink ref="I58" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
updated NGF Round 2 model run log (added 6 more runs)
</commit_message>
<xml_diff>
--- a/utilities/NextGenFwys/ModelRuns_Round2.xlsx
+++ b/utilities/NextGenFwys/ModelRuns_Round2.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atapase\OneDrive - Metropolitan Transportation Commission\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Documents\GitHub\travel-model-one\utilities\NextGenFwys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AB9639-8D04-48CF-9F50-73C8C006DA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2A8D4A-6160-46DA-80FA-E766D6AF08DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_runs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_runs!$A$1:$L$74</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="304">
   <si>
     <t>category</t>
   </si>
@@ -785,12 +786,6 @@
     <t>I:\\Projects\\2035_TM160_NGF_r2_NoProject_06_aoc4.4mb</t>
   </si>
   <si>
-    <t>xxy</t>
-  </si>
-  <si>
-    <t>xxz</t>
-  </si>
-  <si>
     <t>2035_TM160_NGFr2_NP06_Path2_01</t>
   </si>
   <si>
@@ -891,6 +886,69 @@
   </si>
   <si>
     <t>G:\\Projects\\2035_TM160_NGFr2_NP04_Path1_12_highTrnHes</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP07_Path5_01</t>
+  </si>
+  <si>
+    <t>P5 with NP07 (which has lower trn hes than NP04)</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1208104778991669/f</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP07_Path4_01</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1208104778991687/f</t>
+  </si>
+  <si>
+    <t>P4 with NP07 (which has lower trn hes than NP04)</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGFr2_NP07_Path6_01</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_07_aoc2.9cTR</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_07_aoc4.4cTR</t>
+  </si>
+  <si>
+    <t>2035_TM160_NGF_r2_NoProject_07_aoc1.5cTR</t>
+  </si>
+  <si>
+    <t>NoProject_AOCmbuf_TransitRoadway</t>
+  </si>
+  <si>
+    <t>P6 with NP07 (which has lower trn hes than NP04)</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1208104778994762/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/0/1208104778991691/f</t>
+  </si>
+  <si>
+    <t>aoc based mbuf at 7.5c, no cap, network with more transit + road diet</t>
+  </si>
+  <si>
+    <t>aoc based mbuf at 5c, no cap, network with more transit + road diet</t>
+  </si>
+  <si>
+    <t>aoc based mbuf at 2.5c, no cap, network with more transit + road diet</t>
+  </si>
+  <si>
+    <t>NGF_Networks_NGFround2_P2_04</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1208107743449387/f</t>
+  </si>
+  <si>
+    <t>https://app.asana.com/0/1203644633064654/1208107743449388/f</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1094,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1113,6 +1171,9 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1465,11 +1526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2284,7 +2345,7 @@
         <v>2035</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>19</v>
@@ -2293,7 +2354,7 @@
         <v>28</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G25" s="37" t="s">
         <v>31</v>
@@ -2302,12 +2363,12 @@
         <v>224</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>189</v>
@@ -2436,7 +2497,7 @@
         <v>2035</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>19</v>
@@ -2457,7 +2518,7 @@
       <c r="J30" s="34"/>
       <c r="K30" s="34"/>
       <c r="L30" s="32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M30" s="32" t="s">
         <v>189</v>
@@ -2471,7 +2532,7 @@
         <v>2035</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D31" s="32" t="s">
         <v>19</v>
@@ -2486,7 +2547,7 @@
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
       <c r="L31" s="32" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M31" s="32" t="s">
         <v>188</v>
@@ -2500,7 +2561,7 @@
         <v>2035</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D32" s="32" t="s">
         <v>19</v>
@@ -2509,7 +2570,7 @@
         <v>223</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G32" s="35" t="s">
         <v>31</v>
@@ -2518,12 +2579,12 @@
         <v>224</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J32" s="34"/>
       <c r="K32" s="34"/>
       <c r="L32" s="32" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="M32" s="32" t="s">
         <v>188</v>
@@ -2994,7 +3055,7 @@
         <v>2035</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>19</v>
@@ -3002,19 +3063,16 @@
       <c r="E47" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G47" s="36" t="s">
+      <c r="G47" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J47" s="13"/>
       <c r="K47" s="13"/>
       <c r="L47" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M47" s="7" t="s">
         <v>189</v>
@@ -3028,7 +3086,7 @@
         <v>2035</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>19</v>
@@ -3036,19 +3094,16 @@
       <c r="E48" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G48" s="36" t="s">
+      <c r="G48" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="M48" s="7" t="s">
         <v>240</v>
@@ -3073,7 +3128,7 @@
       <c r="F49" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="G49" s="36" t="s">
+      <c r="G49" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H49" s="7" t="s">
@@ -3089,7 +3144,7 @@
         <v>10</v>
       </c>
       <c r="L49" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M49" s="7" t="s">
         <v>193</v>
@@ -3114,7 +3169,6 @@
       <c r="F50" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G50" s="36"/>
       <c r="H50" s="7" t="s">
         <v>108</v>
       </c>
@@ -3145,16 +3199,16 @@
         <v>69</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="G51" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="G51" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J51" s="13"/>
       <c r="K51" s="13"/>
@@ -3180,9 +3234,6 @@
       </c>
       <c r="E52" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>249</v>
       </c>
       <c r="G52" s="36"/>
       <c r="J52" s="13"/>
@@ -3210,9 +3261,6 @@
       <c r="E53" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="7" t="s">
-        <v>250</v>
-      </c>
       <c r="G53" s="36"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
@@ -3231,7 +3279,7 @@
         <v>2035</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>19</v>
@@ -3240,16 +3288,16 @@
         <v>69</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G54" s="36" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
@@ -3262,7 +3310,7 @@
         <v>2035</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>19</v>
@@ -3271,21 +3319,21 @@
         <v>69</v>
       </c>
       <c r="F55" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="G55" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>268</v>
-      </c>
       <c r="I55" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J55" s="13"/>
       <c r="K55" s="13"/>
       <c r="L55" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M55" s="7" t="s">
         <v>189</v>
@@ -3299,7 +3347,7 @@
         <v>2035</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>19</v>
@@ -3308,21 +3356,21 @@
         <v>69</v>
       </c>
       <c r="F56" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="I56" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="G56" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="I56" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="J56" s="13"/>
       <c r="K56" s="13"/>
       <c r="L56" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M56" s="7" t="s">
         <v>193</v>
@@ -3336,7 +3384,7 @@
         <v>2035</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>19</v>
@@ -3345,124 +3393,112 @@
         <v>69</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="G57" s="36" t="s">
-        <v>272</v>
+        <v>271</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
     </row>
-    <row r="58" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F58" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="I58" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J58" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K58" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B59" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D59" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F59" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H59" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I59" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="J59" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K59" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="16">
-        <v>2035</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F60" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="I60" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="J60" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K60" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L60" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="M60" s="15" t="s">
-        <v>190</v>
-      </c>
+    <row r="58" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="G58" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+    </row>
+    <row r="59" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G59" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+    </row>
+    <row r="60" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="8">
+        <v>2035</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="G60" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
     </row>
     <row r="61" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
@@ -3472,7 +3508,7 @@
         <v>2035</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>19</v>
@@ -3481,13 +3517,13 @@
         <v>91</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>148</v>
+        <v>83</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="I61" s="18" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="J61" s="17" t="s">
         <v>10</v>
@@ -3504,7 +3540,7 @@
         <v>2035</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>19</v>
@@ -3513,13 +3549,13 @@
         <v>91</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="J62" s="17" t="s">
         <v>10</v>
@@ -3536,7 +3572,7 @@
         <v>2035</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>19</v>
@@ -3548,286 +3584,290 @@
         <v>126</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>152</v>
+        <v>31</v>
       </c>
       <c r="H63" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="I63" s="18"/>
+      <c r="I63" s="18" t="s">
+        <v>129</v>
+      </c>
       <c r="J63" s="17" t="s">
         <v>10</v>
       </c>
       <c r="K63" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C64" s="27" t="s">
+      <c r="L63" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="M63" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I64" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J64" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K64" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I65" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J65" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K65" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G66" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I66" s="18"/>
+      <c r="J66" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K66" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="16">
+        <v>2035</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="G67" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I67" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+    </row>
+    <row r="68" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C68" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D64" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E64" s="25" t="s">
+      <c r="D68" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="F64" s="25" t="s">
+      <c r="F68" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="H64" s="27" t="s">
+      <c r="H68" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="I64" s="27" t="s">
+      <c r="I68" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="J64" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K64" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B65" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C65" s="27" t="s">
+      <c r="J68" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K68" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C69" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D65" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E65" s="25" t="s">
+      <c r="D69" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="F65" s="25" t="s">
+      <c r="F69" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H65" s="27" t="s">
+      <c r="H69" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="I65" s="27" t="s">
+      <c r="I69" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="J65" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K65" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="26">
-        <v>2035</v>
-      </c>
-      <c r="C66" s="27" t="s">
+      <c r="J69" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K69" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C70" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D66" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E66" s="25" t="s">
+      <c r="D70" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="F66" s="25" t="s">
+      <c r="F70" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="G66" s="27" t="s">
+      <c r="G70" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="H66" s="27" t="s">
+      <c r="H70" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I66" s="27" t="s">
+      <c r="I70" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="J66" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K66" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="L66" s="27" t="s">
+      <c r="J70" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K70" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L70" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="M66" s="27" t="s">
+      <c r="M70" s="27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B67" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C67" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D67" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F67" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H67" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="I67" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="J67" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K67" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B68" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C68" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D68" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E68" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F68" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="H68" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I68" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="J68" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K68" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C69" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="D69" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E69" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F69" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="H69" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="I69" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="J69" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K69" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="L69" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="M69" s="29" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B70" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C70" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E70" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F70" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="H70" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="I70" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="J70" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K70" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" s="30">
-        <v>2035</v>
-      </c>
-      <c r="C71" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="D71" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E71" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F71" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="H71" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="J71" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K71" s="31" t="s">
-        <v>10</v>
-      </c>
+    <row r="71" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="26">
+        <v>2035</v>
+      </c>
+      <c r="C71" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F71" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="G71" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="H71" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="I71" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="J71" s="28"/>
+      <c r="K71" s="28"/>
     </row>
     <row r="72" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="29" t="s">
@@ -3837,7 +3877,7 @@
         <v>2035</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="D72" s="29" t="s">
         <v>19</v>
@@ -3846,34 +3886,228 @@
         <v>117</v>
       </c>
       <c r="F72" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H72" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="I72" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="J72" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K72" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C73" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D73" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F73" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H73" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="I73" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="J73" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K73" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C74" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F74" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="G72" s="29" t="s">
+      <c r="H74" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="I74" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="J74" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K74" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L74" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M74" s="29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C75" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F75" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H75" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="I75" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J75" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K75" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C76" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D76" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F76" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H76" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="J76" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K76" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C77" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F77" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G77" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H72" s="29" t="s">
+      <c r="H77" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="J72" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K72" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="L72" s="29" t="s">
+      <c r="J77" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K77" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L77" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="M72" s="29" t="s">
+      <c r="M77" s="29" t="s">
         <v>191</v>
       </c>
     </row>
+    <row r="78" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" s="30">
+        <v>2035</v>
+      </c>
+      <c r="C78" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="D78" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E78" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F78" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="G78" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="H78" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="I78" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="J78" s="31"/>
+      <c r="K78" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" xr:uid="{2F5DF9E8-6F7C-49D0-A88D-920944076562}"/>
     <hyperlink ref="I13" r:id="rId2" xr:uid="{088533EE-4DDB-4145-8A51-9A459A5B0EE7}"/>
-    <hyperlink ref="I58" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
+    <hyperlink ref="I61" r:id="rId3" xr:uid="{7568B75C-5EC3-4B27-BBC3-154FC1450F6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>